<commit_message>
Errorr en puntuaciones de 400
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cp\Documents\GitHub\DecatlonEstadistics\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F87333-AB65-4D14-A383-A805724920EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385A7A07-3B14-4C63-935E-DFED122868FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3204,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q197" sqref="Q197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20041,7 +20041,7 @@
         <v>835</v>
       </c>
       <c r="Q196">
-        <v>1.0249999999999999</v>
+        <v>1025</v>
       </c>
       <c r="R196">
         <v>14.95</v>

</xml_diff>